<commit_message>
interpolated the groundwater data
finally!!!!!!
</commit_message>
<xml_diff>
--- a/GW-Hyporheic/interpolation_tests.xlsx
+++ b/GW-Hyporheic/interpolation_tests.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huck4481\Documents\GitHub\La_Jara\GW-Hyporheic\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2A594A1B-FDCC-4E5C-9334-D69F1B9F3024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6769210F-4410-4DFB-BFA1-675AE2829334}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" xr2:uid="{4428CE88-35F4-4141-9A43-3E879D4749DC}"/>
+    <workbookView xWindow="-25320" yWindow="195" windowWidth="25440" windowHeight="15390" activeTab="3" xr2:uid="{4428CE88-35F4-4141-9A43-3E879D4749DC}"/>
   </bookViews>
   <sheets>
     <sheet name="tiempo 1" sheetId="1" r:id="rId1"/>
     <sheet name="tiempo 2" sheetId="2" r:id="rId2"/>
     <sheet name="tiempo final" sheetId="3" r:id="rId3"/>
+    <sheet name="SM22 (smth weird is happening)" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="8">
   <si>
     <t xml:space="preserve">Distance (m) </t>
   </si>
@@ -148,7 +149,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -176,6 +177,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -2888,8 +2892,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{867A546B-278B-46C6-A858-20408C3448CF}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="F26" sqref="F26"/>
+    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3033,7 +3037,7 @@
         <v>2721.8069999999998</v>
       </c>
       <c r="D9" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A9,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" ref="D9:D34" si="1">_xlfn.FORECAST.LINEAR(A9,$H$2:$H$3,$I$2:$I$3)</f>
         <v>2721.4793814964028</v>
       </c>
     </row>
@@ -3045,7 +3049,7 @@
         <v>2721.8820000000001</v>
       </c>
       <c r="D10" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A10,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.5174237410074</v>
       </c>
     </row>
@@ -3057,7 +3061,7 @@
         <v>2721.962</v>
       </c>
       <c r="D11" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A11,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.54278523741</v>
       </c>
     </row>
@@ -3069,7 +3073,7 @@
         <v>2721.962</v>
       </c>
       <c r="D12" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A12,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.5744871079137</v>
       </c>
     </row>
@@ -3081,7 +3085,7 @@
         <v>2722.0120000000002</v>
       </c>
       <c r="D13" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A13,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.6061889784173</v>
       </c>
     </row>
@@ -3093,7 +3097,7 @@
         <v>2722.047</v>
       </c>
       <c r="D14" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A14,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.637890848921</v>
       </c>
     </row>
@@ -3105,7 +3109,7 @@
         <v>2722.0619999999999</v>
       </c>
       <c r="D15" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A15,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.6695927194246</v>
       </c>
     </row>
@@ -3117,7 +3121,7 @@
         <v>2722.0970000000002</v>
       </c>
       <c r="D16" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A16,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.7012945899282</v>
       </c>
     </row>
@@ -3129,7 +3133,7 @@
         <v>2722.152</v>
       </c>
       <c r="D17" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A17,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.7329964604319</v>
       </c>
     </row>
@@ -3141,7 +3145,7 @@
         <v>2722.1320000000001</v>
       </c>
       <c r="D18" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A18,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.7646983309355</v>
       </c>
     </row>
@@ -3153,7 +3157,7 @@
         <v>2722.1419999999998</v>
       </c>
       <c r="D19" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A19,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.7964002014387</v>
       </c>
     </row>
@@ -3165,7 +3169,7 @@
         <v>2722.2170000000001</v>
       </c>
       <c r="D20" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A20,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.8281020719423</v>
       </c>
     </row>
@@ -3177,7 +3181,7 @@
         <v>2722.1819999999998</v>
       </c>
       <c r="D21" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A21,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.859803942446</v>
       </c>
     </row>
@@ -3189,7 +3193,7 @@
         <v>2722.2170000000001</v>
       </c>
       <c r="D22" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A22,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.8915058129496</v>
       </c>
     </row>
@@ -3201,7 +3205,7 @@
         <v>2722.2919999999999</v>
       </c>
       <c r="D23" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A23,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.9358884316548</v>
       </c>
     </row>
@@ -3213,7 +3217,7 @@
         <v>2722.3420000000001</v>
       </c>
       <c r="D24" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A24,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2721.9866114244605</v>
       </c>
     </row>
@@ -3225,7 +3229,7 @@
         <v>2722.4319999999998</v>
       </c>
       <c r="D25" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A25,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2722.0056325467626</v>
       </c>
     </row>
@@ -3237,7 +3241,7 @@
         <v>2722.4920000000002</v>
       </c>
       <c r="D26" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A26,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2722.0500151654678</v>
       </c>
     </row>
@@ -3249,7 +3253,7 @@
         <v>2722.4720000000002</v>
       </c>
       <c r="D27" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A27,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2722.0817170359715</v>
       </c>
     </row>
@@ -3261,7 +3265,7 @@
         <v>2722.4870000000001</v>
       </c>
       <c r="D28" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A28,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2722.1134189064746</v>
       </c>
     </row>
@@ -3273,7 +3277,7 @@
         <v>2722.5720000000001</v>
       </c>
       <c r="D29" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A29,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2722.1451207769783</v>
       </c>
     </row>
@@ -3285,7 +3289,7 @@
         <v>2722.6170000000002</v>
       </c>
       <c r="D30" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A30,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2722.1768226474819</v>
       </c>
     </row>
@@ -3297,7 +3301,7 @@
         <v>2722.587</v>
       </c>
       <c r="D31" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A31,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2722.2085245179856</v>
       </c>
     </row>
@@ -3309,7 +3313,7 @@
         <v>2722.587</v>
       </c>
       <c r="D32" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A32,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2722.2402263884892</v>
       </c>
     </row>
@@ -3321,7 +3325,7 @@
         <v>2722.5520000000001</v>
       </c>
       <c r="D33" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A33,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2722.2719282589928</v>
       </c>
     </row>
@@ -3333,7 +3337,7 @@
         <v>2722.5790000000002</v>
       </c>
       <c r="D34" s="3">
-        <f>_xlfn.FORECAST.LINEAR(A34,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" si="1"/>
         <v>2722.3036301294965</v>
       </c>
     </row>
@@ -3371,7 +3375,7 @@
         <v>2722.654</v>
       </c>
       <c r="D37" s="3">
-        <f t="shared" ref="D37:D91" si="1">_xlfn.FORECAST.LINEAR(A37,$H$2:$H$3,$I$2:$I$3)</f>
+        <f t="shared" ref="D37:D91" si="2">_xlfn.FORECAST.LINEAR(A37,$H$2:$H$3,$I$2:$I$3)</f>
         <v>2722.4177568633095</v>
       </c>
     </row>
@@ -3383,7 +3387,7 @@
         <v>2722.779</v>
       </c>
       <c r="D38" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.4367779856116</v>
       </c>
     </row>
@@ -3395,7 +3399,7 @@
         <v>2722.6990000000001</v>
       </c>
       <c r="D39" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.4684798561152</v>
       </c>
     </row>
@@ -3407,7 +3411,7 @@
         <v>2723.0039999999999</v>
       </c>
       <c r="D40" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.4811606043168</v>
       </c>
     </row>
@@ -3419,7 +3423,7 @@
         <v>2723.0239999999999</v>
       </c>
       <c r="D41" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.4938413525178</v>
       </c>
     </row>
@@ -3431,7 +3435,7 @@
         <v>2723.0790000000002</v>
       </c>
       <c r="D42" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.5255432230215</v>
       </c>
     </row>
@@ -3443,7 +3447,7 @@
         <v>2723.0740000000001</v>
       </c>
       <c r="D43" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.5572450935251</v>
       </c>
     </row>
@@ -3455,7 +3459,7 @@
         <v>2723.0039999999999</v>
       </c>
       <c r="D44" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.5699258417267</v>
       </c>
     </row>
@@ -3467,7 +3471,7 @@
         <v>2723.0990000000002</v>
       </c>
       <c r="D45" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.5699258417267</v>
       </c>
     </row>
@@ -3479,7 +3483,7 @@
         <v>2723.049</v>
       </c>
       <c r="D46" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.6143084604319</v>
       </c>
     </row>
@@ -3491,7 +3495,7 @@
         <v>2723.1790000000001</v>
       </c>
       <c r="D47" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.6269892086329</v>
       </c>
     </row>
@@ -3503,7 +3507,7 @@
         <v>2723.1889999999999</v>
       </c>
       <c r="D48" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.6976843798561</v>
       </c>
     </row>
@@ -3515,7 +3519,7 @@
         <v>2723.1689999999999</v>
       </c>
       <c r="D49" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.7157544460433</v>
       </c>
     </row>
@@ -3527,7 +3531,7 @@
         <v>2723.1590000000001</v>
       </c>
       <c r="D50" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.747456316547</v>
       </c>
     </row>
@@ -3539,7 +3543,7 @@
         <v>2723.1489999999999</v>
       </c>
       <c r="D51" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.7791581870506</v>
       </c>
     </row>
@@ -3551,7 +3555,7 @@
         <v>2723.1590000000001</v>
       </c>
       <c r="D52" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.8108600575538</v>
       </c>
     </row>
@@ -3563,7 +3567,7 @@
         <v>2723.239</v>
       </c>
       <c r="D53" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.8425619280574</v>
       </c>
     </row>
@@ -3575,7 +3579,7 @@
         <v>2723.259</v>
       </c>
       <c r="D54" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.8742637985611</v>
       </c>
     </row>
@@ -3587,7 +3591,7 @@
         <v>2723.5189999999998</v>
       </c>
       <c r="D55" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.8996252949642</v>
       </c>
     </row>
@@ -3599,7 +3603,7 @@
         <v>2723.4290000000001</v>
       </c>
       <c r="D56" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.9376675395683</v>
       </c>
     </row>
@@ -3611,7 +3615,7 @@
         <v>2723.4490000000001</v>
       </c>
       <c r="D57" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2722.9630290359714</v>
       </c>
     </row>
@@ -3623,7 +3627,7 @@
         <v>2723.5189999999998</v>
       </c>
       <c r="D58" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.0010712805756</v>
       </c>
     </row>
@@ -3635,7 +3639,7 @@
         <v>2723.6590000000001</v>
       </c>
       <c r="D59" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.0200924028777</v>
       </c>
     </row>
@@ -3647,7 +3651,7 @@
         <v>2723.5790000000002</v>
       </c>
       <c r="D60" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.0327731510793</v>
       </c>
     </row>
@@ -3659,7 +3663,7 @@
         <v>2723.7089999999998</v>
       </c>
       <c r="D61" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.0644750215829</v>
       </c>
     </row>
@@ -3671,7 +3675,7 @@
         <v>2723.6689999999999</v>
       </c>
       <c r="D62" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.0961768920865</v>
       </c>
     </row>
@@ -3683,7 +3687,7 @@
         <v>2723.7089999999998</v>
       </c>
       <c r="D63" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.1278787625897</v>
       </c>
     </row>
@@ -3695,7 +3699,7 @@
         <v>2723.819</v>
       </c>
       <c r="D64" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.1595806330934</v>
       </c>
     </row>
@@ -3707,7 +3711,7 @@
         <v>2723.8389999999999</v>
       </c>
       <c r="D65" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.191282503597</v>
       </c>
     </row>
@@ -3719,7 +3723,7 @@
         <v>2723.8389999999999</v>
       </c>
       <c r="D66" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.2229843741006</v>
       </c>
     </row>
@@ -3731,7 +3735,7 @@
         <v>2723.8789999999999</v>
       </c>
       <c r="D67" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.2546862446043</v>
       </c>
     </row>
@@ -3743,7 +3747,7 @@
         <v>2723.924</v>
       </c>
       <c r="D68" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.2863881151079</v>
       </c>
     </row>
@@ -3755,7 +3759,7 @@
         <v>2723.884</v>
       </c>
       <c r="D69" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.3180899856116</v>
       </c>
     </row>
@@ -3767,7 +3771,7 @@
         <v>2724.0790000000002</v>
       </c>
       <c r="D70" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.3624726043167</v>
       </c>
     </row>
@@ -3779,7 +3783,7 @@
         <v>2724.1640000000002</v>
       </c>
       <c r="D71" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.3814937266188</v>
       </c>
     </row>
@@ -3791,7 +3795,7 @@
         <v>2724.1840000000002</v>
       </c>
       <c r="D72" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.4131955971225</v>
       </c>
     </row>
@@ -3803,7 +3807,7 @@
         <v>2724.2139999999999</v>
       </c>
       <c r="D73" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.4448974676261</v>
       </c>
     </row>
@@ -3815,7 +3819,7 @@
         <v>2724.194</v>
       </c>
       <c r="D74" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.4765993381293</v>
       </c>
     </row>
@@ -3827,7 +3831,7 @@
         <v>2724.2289999999998</v>
       </c>
       <c r="D75" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.4956204604318</v>
       </c>
     </row>
@@ -3839,7 +3843,7 @@
         <v>2724.5540000000001</v>
       </c>
       <c r="D76" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.5019608345324</v>
       </c>
     </row>
@@ -3851,7 +3855,7 @@
         <v>2724.6239999999998</v>
       </c>
       <c r="D77" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.5209819568345</v>
       </c>
     </row>
@@ -3863,7 +3867,7 @@
         <v>2724.5540000000001</v>
       </c>
       <c r="D78" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.5526838273381</v>
       </c>
     </row>
@@ -3875,7 +3879,7 @@
         <v>2724.5839999999998</v>
       </c>
       <c r="D79" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.5717049496402</v>
       </c>
     </row>
@@ -3887,7 +3891,7 @@
         <v>2724.5540000000001</v>
       </c>
       <c r="D80" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.5970664460433</v>
       </c>
     </row>
@@ -3899,7 +3903,7 @@
         <v>2724.5740000000001</v>
       </c>
       <c r="D81" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.6160875683454</v>
       </c>
     </row>
@@ -3911,7 +3915,7 @@
         <v>2724.6039999999998</v>
       </c>
       <c r="D82" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.6351086906475</v>
       </c>
     </row>
@@ -3923,7 +3927,7 @@
         <v>2724.6390000000001</v>
       </c>
       <c r="D83" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.6668105611511</v>
       </c>
     </row>
@@ -3935,7 +3939,7 @@
         <v>2724.6590000000001</v>
       </c>
       <c r="D84" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.6985124316548</v>
       </c>
     </row>
@@ -3947,7 +3951,7 @@
         <v>2724.6439999999998</v>
       </c>
       <c r="D85" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.7302143021584</v>
       </c>
     </row>
@@ -3959,7 +3963,7 @@
         <v>2724.6590000000001</v>
       </c>
       <c r="D86" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.761916172662</v>
       </c>
     </row>
@@ -3971,7 +3975,7 @@
         <v>2724.7440000000001</v>
       </c>
       <c r="D87" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.7745969208631</v>
       </c>
     </row>
@@ -3983,7 +3987,7 @@
         <v>2724.7489999999998</v>
       </c>
       <c r="D88" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.7936180431657</v>
       </c>
     </row>
@@ -3995,7 +3999,7 @@
         <v>2724.7440000000001</v>
       </c>
       <c r="D89" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.8253199136689</v>
       </c>
     </row>
@@ -4007,7 +4011,7 @@
         <v>2724.7139999999999</v>
       </c>
       <c r="D90" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.8570217841725</v>
       </c>
     </row>
@@ -4019,7 +4023,7 @@
         <v>2724.7440000000001</v>
       </c>
       <c r="D91" s="4">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>2723.8887236546761</v>
       </c>
     </row>
@@ -4818,8 +4822,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6325C07-E472-4FD6-8F53-84F07547DE89}">
   <dimension ref="A1:I91"/>
   <sheetViews>
-    <sheetView topLeftCell="A70" workbookViewId="0">
-      <selection activeCell="G91" sqref="G91"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E37" sqref="E37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4839,8 +4843,8 @@
       <c r="G1" s="10">
         <v>44461.989583333336</v>
       </c>
-      <c r="H1" s="9"/>
-      <c r="I1" s="9"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
@@ -4972,7 +4976,7 @@
         <v>2721.8820000000001</v>
       </c>
       <c r="D10">
-        <f t="shared" ref="D10:D34" si="1">_xlfn.FORECAST.LINEAR(A10,$H$3:$H$4,$I$3:$I$4)</f>
+        <f t="shared" ref="D10:D33" si="1">_xlfn.FORECAST.LINEAR(A10,$H$3:$H$4,$I$3:$I$4)</f>
         <v>2721.3835588705033</v>
       </c>
     </row>
@@ -5956,4 +5960,1151 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4C5F628C-98B8-4930-B92A-0C3D12CB8FBB}">
+  <dimension ref="A1:H91"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="13.140625" customWidth="1"/>
+    <col min="2" max="2" width="15.42578125" customWidth="1"/>
+    <col min="4" max="4" width="20.5703125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="10">
+        <v>44772</v>
+      </c>
+      <c r="D1" s="10"/>
+      <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="9">
+        <v>0</v>
+      </c>
+      <c r="B2" s="9">
+        <v>2721.752</v>
+      </c>
+      <c r="D2">
+        <f>_xlfn.FORECAST.LINEAR(A2,$G$2:$G$3,$H$2:$H$3)</f>
+        <v>2721.1612571654678</v>
+      </c>
+      <c r="F2" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>2721.347397</v>
+      </c>
+      <c r="H2">
+        <f>A8</f>
+        <v>3.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="9">
+        <v>0.3</v>
+      </c>
+      <c r="B3" s="9">
+        <v>2721.7420000000002</v>
+      </c>
+      <c r="D3">
+        <f t="shared" ref="D3:D6" si="0">_xlfn.FORECAST.LINEAR(A3,$G$2:$G$3,$H$2:$H$3)</f>
+        <v>2721.1792706978417</v>
+      </c>
+      <c r="F3" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="G3">
+        <v>2722.1820240000002</v>
+      </c>
+      <c r="H3">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A4" s="9">
+        <v>1</v>
+      </c>
+      <c r="B4" s="9">
+        <v>2721.7620000000002</v>
+      </c>
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>2721.2213022733813</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A5" s="9">
+        <v>1.5</v>
+      </c>
+      <c r="B5" s="9">
+        <v>2721.732</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>2721.2513248273381</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A6" s="9">
+        <v>2</v>
+      </c>
+      <c r="B6" s="9">
+        <v>2721.732</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="0"/>
+        <v>2721.2813473812953</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A7" s="9">
+        <v>2.5</v>
+      </c>
+      <c r="B7" s="9">
+        <v>2721.7620000000002</v>
+      </c>
+      <c r="D7">
+        <f>_xlfn.FORECAST.LINEAR(A7,$G$2:$G$3,$H$2:$H$3)</f>
+        <v>2721.3113699352521</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A8" s="9">
+        <v>3.1</v>
+      </c>
+      <c r="B8" s="9">
+        <v>2721.7820000000002</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="D8" s="8">
+        <f>_xlfn.FORECAST.LINEAR(A8,$G$2:$G$3,$H$2:$H$3)</f>
+        <v>2721.347397</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A9" s="9">
+        <v>3.5</v>
+      </c>
+      <c r="B9" s="9">
+        <v>2721.8069999999998</v>
+      </c>
+      <c r="D9">
+        <f t="shared" ref="D9:D34" si="1">_xlfn.FORECAST.LINEAR(A9,$G$2:$G$3,$H$2:$H$3)</f>
+        <v>2721.3714150431656</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" s="9">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="B10" s="9">
+        <v>2721.8820000000001</v>
+      </c>
+      <c r="D10">
+        <f t="shared" si="1"/>
+        <v>2721.407442107914</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A11" s="9">
+        <v>4.5</v>
+      </c>
+      <c r="B11" s="9">
+        <v>2721.962</v>
+      </c>
+      <c r="D11">
+        <f t="shared" si="1"/>
+        <v>2721.4314601510791</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A12" s="9">
+        <v>5</v>
+      </c>
+      <c r="B12" s="9">
+        <v>2721.962</v>
+      </c>
+      <c r="D12">
+        <f t="shared" si="1"/>
+        <v>2721.4614827050364</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A13" s="9">
+        <v>5.5</v>
+      </c>
+      <c r="B13" s="9">
+        <v>2722.0120000000002</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="1"/>
+        <v>2721.4915052589931</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A14" s="9">
+        <v>6</v>
+      </c>
+      <c r="B14" s="9">
+        <v>2722.047</v>
+      </c>
+      <c r="D14">
+        <f t="shared" si="1"/>
+        <v>2721.5215278129499</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A15" s="9">
+        <v>6.5</v>
+      </c>
+      <c r="B15" s="9">
+        <v>2722.0619999999999</v>
+      </c>
+      <c r="D15">
+        <f t="shared" si="1"/>
+        <v>2721.5515503669067</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16" s="9">
+        <v>7</v>
+      </c>
+      <c r="B16" s="9">
+        <v>2722.0970000000002</v>
+      </c>
+      <c r="D16">
+        <f t="shared" si="1"/>
+        <v>2721.5815729208634</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="9">
+        <v>7.5</v>
+      </c>
+      <c r="B17" s="9">
+        <v>2722.152</v>
+      </c>
+      <c r="D17">
+        <f t="shared" si="1"/>
+        <v>2721.6115954748202</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="9">
+        <v>8</v>
+      </c>
+      <c r="B18" s="9">
+        <v>2722.1320000000001</v>
+      </c>
+      <c r="D18">
+        <f t="shared" si="1"/>
+        <v>2721.6416180287774</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="9">
+        <v>8.5</v>
+      </c>
+      <c r="B19" s="9">
+        <v>2722.1419999999998</v>
+      </c>
+      <c r="D19">
+        <f t="shared" si="1"/>
+        <v>2721.6716405827342</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="9">
+        <v>9</v>
+      </c>
+      <c r="B20" s="9">
+        <v>2722.2170000000001</v>
+      </c>
+      <c r="D20">
+        <f t="shared" si="1"/>
+        <v>2721.701663136691</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="9">
+        <v>9.5</v>
+      </c>
+      <c r="B21" s="9">
+        <v>2722.1819999999998</v>
+      </c>
+      <c r="D21">
+        <f t="shared" si="1"/>
+        <v>2721.7316856906477</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="9">
+        <v>10</v>
+      </c>
+      <c r="B22" s="9">
+        <v>2722.2170000000001</v>
+      </c>
+      <c r="D22">
+        <f t="shared" si="1"/>
+        <v>2721.7617082446045</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="9">
+        <v>10.7</v>
+      </c>
+      <c r="B23" s="9">
+        <v>2722.2919999999999</v>
+      </c>
+      <c r="D23">
+        <f t="shared" si="1"/>
+        <v>2721.8037398201441</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="9">
+        <v>11.5</v>
+      </c>
+      <c r="B24" s="9">
+        <v>2722.3420000000001</v>
+      </c>
+      <c r="D24">
+        <f t="shared" si="1"/>
+        <v>2721.8517759064753</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="9">
+        <v>11.8</v>
+      </c>
+      <c r="B25" s="9">
+        <v>2722.4319999999998</v>
+      </c>
+      <c r="D25">
+        <f t="shared" si="1"/>
+        <v>2721.8697894388492</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="9">
+        <v>12.5</v>
+      </c>
+      <c r="B26" s="9">
+        <v>2722.4920000000002</v>
+      </c>
+      <c r="D26">
+        <f t="shared" si="1"/>
+        <v>2721.9118210143888</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="9">
+        <v>13</v>
+      </c>
+      <c r="B27" s="9">
+        <v>2722.4720000000002</v>
+      </c>
+      <c r="D27">
+        <f t="shared" si="1"/>
+        <v>2721.9418435683456</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="9">
+        <v>13.5</v>
+      </c>
+      <c r="B28" s="9">
+        <v>2722.4870000000001</v>
+      </c>
+      <c r="D28">
+        <f t="shared" si="1"/>
+        <v>2721.9718661223023</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="9">
+        <v>14</v>
+      </c>
+      <c r="B29" s="9">
+        <v>2722.5720000000001</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="1"/>
+        <v>2722.0018886762591</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="9">
+        <v>14.5</v>
+      </c>
+      <c r="B30" s="9">
+        <v>2722.6170000000002</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="1"/>
+        <v>2722.0319112302163</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="9">
+        <v>15</v>
+      </c>
+      <c r="B31" s="9">
+        <v>2722.587</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="1"/>
+        <v>2722.0619337841731</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="9">
+        <v>15.5</v>
+      </c>
+      <c r="B32" s="9">
+        <v>2722.587</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="1"/>
+        <v>2722.0919563381299</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="9">
+        <v>16</v>
+      </c>
+      <c r="B33" s="9">
+        <v>2722.5520000000001</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="1"/>
+        <v>2722.1219788920866</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A34" s="9">
+        <v>16.5</v>
+      </c>
+      <c r="B34" s="9">
+        <v>2722.5790000000002</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>2722.1520014460434</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="9">
+        <v>17</v>
+      </c>
+      <c r="B35" s="9">
+        <v>2722.5619999999999</v>
+      </c>
+      <c r="C35" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="D35" s="8">
+        <f>_xlfn.FORECAST.LINEAR(A35,$G$2:$G$3,$H$2:$H$3)</f>
+        <v>2722.1820240000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="9">
+        <v>17.5</v>
+      </c>
+      <c r="B36" s="9">
+        <v>2722.652</v>
+      </c>
+      <c r="D36">
+        <f>_xlfn.FORECAST.LINEAR(A36,$G$2:$G$3,$H$2:$H$3)</f>
+        <v>2722.2120465539574</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="9">
+        <v>18.3</v>
+      </c>
+      <c r="B37" s="9">
+        <v>2722.654</v>
+      </c>
+      <c r="D37">
+        <f t="shared" ref="D37:D91" si="2">_xlfn.FORECAST.LINEAR(A37,$G$2:$G$3,$H$2:$H$3)</f>
+        <v>2722.2600826402881</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="9">
+        <v>18.600000000000001</v>
+      </c>
+      <c r="B38" s="9">
+        <v>2722.779</v>
+      </c>
+      <c r="D38">
+        <f t="shared" si="2"/>
+        <v>2722.2780961726621</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="9">
+        <v>19.100000000000001</v>
+      </c>
+      <c r="B39" s="9">
+        <v>2722.6990000000001</v>
+      </c>
+      <c r="D39">
+        <f t="shared" si="2"/>
+        <v>2722.3081187266189</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="9">
+        <v>19.3</v>
+      </c>
+      <c r="B40" s="9">
+        <v>2723.0039999999999</v>
+      </c>
+      <c r="D40">
+        <f t="shared" si="2"/>
+        <v>2722.3201277482017</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="9">
+        <v>19.5</v>
+      </c>
+      <c r="B41" s="9">
+        <v>2723.0239999999999</v>
+      </c>
+      <c r="D41">
+        <f t="shared" si="2"/>
+        <v>2722.3321367697845</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="9">
+        <v>20</v>
+      </c>
+      <c r="B42" s="9">
+        <v>2723.0790000000002</v>
+      </c>
+      <c r="D42">
+        <f t="shared" si="2"/>
+        <v>2722.3621593237413</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A43" s="9">
+        <v>20.5</v>
+      </c>
+      <c r="B43" s="9">
+        <v>2723.0740000000001</v>
+      </c>
+      <c r="D43">
+        <f t="shared" si="2"/>
+        <v>2722.392181877698</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="9">
+        <v>20.7</v>
+      </c>
+      <c r="B44" s="9">
+        <v>2723.0039999999999</v>
+      </c>
+      <c r="D44">
+        <f t="shared" si="2"/>
+        <v>2722.4041908992808</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A45" s="9">
+        <v>20.7</v>
+      </c>
+      <c r="B45" s="9">
+        <v>2723.0990000000002</v>
+      </c>
+      <c r="D45">
+        <f t="shared" si="2"/>
+        <v>2722.4041908992808</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" s="9">
+        <v>21.4</v>
+      </c>
+      <c r="B46" s="9">
+        <v>2723.049</v>
+      </c>
+      <c r="D46">
+        <f t="shared" si="2"/>
+        <v>2722.4462224748204</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" s="9">
+        <v>21.6</v>
+      </c>
+      <c r="B47" s="9">
+        <v>2723.1790000000001</v>
+      </c>
+      <c r="D47">
+        <f t="shared" si="2"/>
+        <v>2722.4582314964032</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A48" s="9">
+        <v>22.715</v>
+      </c>
+      <c r="B48" s="9">
+        <v>2723.1889999999999</v>
+      </c>
+      <c r="D48">
+        <f t="shared" si="2"/>
+        <v>2722.5251817917269</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A49" s="9">
+        <v>23</v>
+      </c>
+      <c r="B49" s="9">
+        <v>2723.1689999999999</v>
+      </c>
+      <c r="D49">
+        <f t="shared" si="2"/>
+        <v>2722.5422946474823</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A50" s="9">
+        <v>23.5</v>
+      </c>
+      <c r="B50" s="9">
+        <v>2723.1590000000001</v>
+      </c>
+      <c r="D50">
+        <f t="shared" si="2"/>
+        <v>2722.5723172014391</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A51" s="9">
+        <v>24</v>
+      </c>
+      <c r="B51" s="9">
+        <v>2723.1489999999999</v>
+      </c>
+      <c r="D51">
+        <f t="shared" si="2"/>
+        <v>2722.6023397553963</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A52" s="9">
+        <v>24.5</v>
+      </c>
+      <c r="B52" s="9">
+        <v>2723.1590000000001</v>
+      </c>
+      <c r="D52">
+        <f t="shared" si="2"/>
+        <v>2722.6323623093531</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A53" s="9">
+        <v>25</v>
+      </c>
+      <c r="B53" s="9">
+        <v>2723.239</v>
+      </c>
+      <c r="D53">
+        <f t="shared" si="2"/>
+        <v>2722.6623848633099</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A54" s="9">
+        <v>25.5</v>
+      </c>
+      <c r="B54" s="9">
+        <v>2723.259</v>
+      </c>
+      <c r="D54">
+        <f t="shared" si="2"/>
+        <v>2722.6924074172666</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A55" s="9">
+        <v>25.9</v>
+      </c>
+      <c r="B55" s="9">
+        <v>2723.5189999999998</v>
+      </c>
+      <c r="D55">
+        <f t="shared" si="2"/>
+        <v>2722.7164254604322</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A56" s="9">
+        <v>26.5</v>
+      </c>
+      <c r="B56" s="9">
+        <v>2723.4290000000001</v>
+      </c>
+      <c r="D56">
+        <f t="shared" si="2"/>
+        <v>2722.7524525251802</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A57" s="9">
+        <v>26.9</v>
+      </c>
+      <c r="B57" s="9">
+        <v>2723.4490000000001</v>
+      </c>
+      <c r="D57">
+        <f t="shared" si="2"/>
+        <v>2722.7764705683458</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A58" s="9">
+        <v>27.5</v>
+      </c>
+      <c r="B58" s="9">
+        <v>2723.5189999999998</v>
+      </c>
+      <c r="D58">
+        <f t="shared" si="2"/>
+        <v>2722.8124976330942</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A59" s="9">
+        <v>27.8</v>
+      </c>
+      <c r="B59" s="9">
+        <v>2723.6590000000001</v>
+      </c>
+      <c r="D59">
+        <f t="shared" si="2"/>
+        <v>2722.8305111654681</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A60" s="9">
+        <v>28</v>
+      </c>
+      <c r="B60" s="9">
+        <v>2723.5790000000002</v>
+      </c>
+      <c r="D60">
+        <f t="shared" si="2"/>
+        <v>2722.8425201870509</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" s="9">
+        <v>28.5</v>
+      </c>
+      <c r="B61" s="9">
+        <v>2723.7089999999998</v>
+      </c>
+      <c r="D61">
+        <f t="shared" si="2"/>
+        <v>2722.8725427410077</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A62" s="9">
+        <v>29</v>
+      </c>
+      <c r="B62" s="9">
+        <v>2723.6689999999999</v>
+      </c>
+      <c r="D62">
+        <f t="shared" si="2"/>
+        <v>2722.9025652949645</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A63" s="9">
+        <v>29.5</v>
+      </c>
+      <c r="B63" s="9">
+        <v>2723.7089999999998</v>
+      </c>
+      <c r="D63">
+        <f t="shared" si="2"/>
+        <v>2722.9325878489212</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A64" s="9">
+        <v>30</v>
+      </c>
+      <c r="B64" s="9">
+        <v>2723.819</v>
+      </c>
+      <c r="D64">
+        <f t="shared" si="2"/>
+        <v>2722.962610402878</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A65" s="9">
+        <v>30.5</v>
+      </c>
+      <c r="B65" s="9">
+        <v>2723.8389999999999</v>
+      </c>
+      <c r="D65">
+        <f t="shared" si="2"/>
+        <v>2722.9926329568352</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="9">
+        <v>31</v>
+      </c>
+      <c r="B66" s="9">
+        <v>2723.8389999999999</v>
+      </c>
+      <c r="D66">
+        <f t="shared" si="2"/>
+        <v>2723.022655510792</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" s="9">
+        <v>31.5</v>
+      </c>
+      <c r="B67" s="9">
+        <v>2723.8789999999999</v>
+      </c>
+      <c r="D67">
+        <f t="shared" si="2"/>
+        <v>2723.0526780647488</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" s="9">
+        <v>32</v>
+      </c>
+      <c r="B68" s="9">
+        <v>2723.924</v>
+      </c>
+      <c r="D68">
+        <f t="shared" si="2"/>
+        <v>2723.0827006187055</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A69" s="9">
+        <v>32.5</v>
+      </c>
+      <c r="B69" s="9">
+        <v>2723.884</v>
+      </c>
+      <c r="D69">
+        <f t="shared" si="2"/>
+        <v>2723.1127231726623</v>
+      </c>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A70" s="9">
+        <v>33.200000000000003</v>
+      </c>
+      <c r="B70" s="9">
+        <v>2724.0790000000002</v>
+      </c>
+      <c r="D70">
+        <f t="shared" si="2"/>
+        <v>2723.1547547482019</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A71" s="9">
+        <v>33.5</v>
+      </c>
+      <c r="B71" s="9">
+        <v>2724.1640000000002</v>
+      </c>
+      <c r="D71">
+        <f t="shared" si="2"/>
+        <v>2723.1727682805763</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A72" s="9">
+        <v>34</v>
+      </c>
+      <c r="B72" s="9">
+        <v>2724.1840000000002</v>
+      </c>
+      <c r="D72">
+        <f t="shared" si="2"/>
+        <v>2723.2027908345331</v>
+      </c>
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A73" s="9">
+        <v>34.5</v>
+      </c>
+      <c r="B73" s="9">
+        <v>2724.2139999999999</v>
+      </c>
+      <c r="D73">
+        <f t="shared" si="2"/>
+        <v>2723.2328133884898</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A74" s="9">
+        <v>35</v>
+      </c>
+      <c r="B74" s="9">
+        <v>2724.194</v>
+      </c>
+      <c r="D74">
+        <f t="shared" si="2"/>
+        <v>2723.2628359424466</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A75" s="9">
+        <v>35.299999999999997</v>
+      </c>
+      <c r="B75" s="9">
+        <v>2724.2289999999998</v>
+      </c>
+      <c r="D75">
+        <f t="shared" si="2"/>
+        <v>2723.2808494748206</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A76" s="9">
+        <v>35.4</v>
+      </c>
+      <c r="B76" s="9">
+        <v>2724.5540000000001</v>
+      </c>
+      <c r="D76">
+        <f t="shared" si="2"/>
+        <v>2723.2868539856122</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="9">
+        <v>35.700000000000003</v>
+      </c>
+      <c r="B77" s="9">
+        <v>2724.6239999999998</v>
+      </c>
+      <c r="D77">
+        <f t="shared" si="2"/>
+        <v>2723.3048675179862</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" s="9">
+        <v>36.200000000000003</v>
+      </c>
+      <c r="B78" s="9">
+        <v>2724.5540000000001</v>
+      </c>
+      <c r="D78">
+        <f t="shared" si="2"/>
+        <v>2723.3348900719429</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" s="9">
+        <v>36.5</v>
+      </c>
+      <c r="B79" s="9">
+        <v>2724.5839999999998</v>
+      </c>
+      <c r="D79">
+        <f t="shared" si="2"/>
+        <v>2723.3529036043174</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A80" s="9">
+        <v>36.9</v>
+      </c>
+      <c r="B80" s="9">
+        <v>2724.5540000000001</v>
+      </c>
+      <c r="D80">
+        <f t="shared" si="2"/>
+        <v>2723.3769216474825</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A81" s="9">
+        <v>37.200000000000003</v>
+      </c>
+      <c r="B81" s="9">
+        <v>2724.5740000000001</v>
+      </c>
+      <c r="D81">
+        <f t="shared" si="2"/>
+        <v>2723.3949351798569</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A82" s="9">
+        <v>37.5</v>
+      </c>
+      <c r="B82" s="9">
+        <v>2724.6039999999998</v>
+      </c>
+      <c r="D82">
+        <f t="shared" si="2"/>
+        <v>2723.4129487122309</v>
+      </c>
+    </row>
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A83" s="9">
+        <v>38</v>
+      </c>
+      <c r="B83" s="9">
+        <v>2724.6390000000001</v>
+      </c>
+      <c r="D83">
+        <f t="shared" si="2"/>
+        <v>2723.4429712661877</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="9">
+        <v>38.5</v>
+      </c>
+      <c r="B84" s="9">
+        <v>2724.6590000000001</v>
+      </c>
+      <c r="D84">
+        <f t="shared" si="2"/>
+        <v>2723.4729938201444</v>
+      </c>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" s="9">
+        <v>39</v>
+      </c>
+      <c r="B85" s="9">
+        <v>2724.6439999999998</v>
+      </c>
+      <c r="D85">
+        <f t="shared" si="2"/>
+        <v>2723.5030163741012</v>
+      </c>
+    </row>
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" s="9">
+        <v>39.5</v>
+      </c>
+      <c r="B86" s="9">
+        <v>2724.6590000000001</v>
+      </c>
+      <c r="D86">
+        <f t="shared" si="2"/>
+        <v>2723.5330389280584</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A87" s="9">
+        <v>39.700000000000003</v>
+      </c>
+      <c r="B87" s="9">
+        <v>2724.7440000000001</v>
+      </c>
+      <c r="D87">
+        <f t="shared" si="2"/>
+        <v>2723.5450479496408</v>
+      </c>
+    </row>
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A88" s="9">
+        <v>40</v>
+      </c>
+      <c r="B88" s="9">
+        <v>2724.7489999999998</v>
+      </c>
+      <c r="D88">
+        <f t="shared" si="2"/>
+        <v>2723.5630614820152</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A89" s="9">
+        <v>40.5</v>
+      </c>
+      <c r="B89" s="9">
+        <v>2724.7440000000001</v>
+      </c>
+      <c r="D89">
+        <f t="shared" si="2"/>
+        <v>2723.593084035972</v>
+      </c>
+    </row>
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A90" s="9">
+        <v>41</v>
+      </c>
+      <c r="B90" s="9">
+        <v>2724.7139999999999</v>
+      </c>
+      <c r="D90">
+        <f t="shared" si="2"/>
+        <v>2723.6231065899287</v>
+      </c>
+    </row>
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A91" s="9">
+        <v>41.5</v>
+      </c>
+      <c r="B91" s="9">
+        <v>2724.7440000000001</v>
+      </c>
+      <c r="D91">
+        <f t="shared" si="2"/>
+        <v>2723.6531291438855</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C1:D1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>